<commit_message>
Debugs faculty performance excel
* removes 'not available' from faculty excel
* removes unnecessary requirements
</commit_message>
<xml_diff>
--- a/Section-Faculty Information/subject_section_faculty_even_sem_2016.xlsx
+++ b/Section-Faculty Information/subject_section_faculty_even_sem_2016.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="980" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1599" uniqueCount="456">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1599" uniqueCount="455">
   <si>
     <t xml:space="preserve">EOE-081</t>
   </si>
@@ -1213,7 +1213,7 @@
     <t xml:space="preserve">DR.M.K.GOYAL</t>
   </si>
   <si>
-    <t xml:space="preserve">DR.ABHISHEK PATHAK     S/I</t>
+    <t xml:space="preserve">DR.ABHISHEK PATHAK</t>
   </si>
   <si>
     <t xml:space="preserve">DR.PARUL VERMA</t>
@@ -1256,7 +1256,7 @@
     <t xml:space="preserve">NAS-205</t>
   </si>
   <si>
-    <t xml:space="preserve">DR.SANDEEP GUPTA    S/I</t>
+    <t xml:space="preserve">DR.SANDEEP GUPTA</t>
   </si>
   <si>
     <t xml:space="preserve">NME-202</t>
@@ -1309,9 +1309,6 @@
   </si>
   <si>
     <t xml:space="preserve">DR.NEETU SHARMA    S/I</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DR.SANDEEP GUPTA</t>
   </si>
   <si>
     <t xml:space="preserve">MR.GAJESH CHAUHAN</t>
@@ -2014,16 +2011,16 @@
   </sheetPr>
   <dimension ref="A2:F538"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A408" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B312" activeCellId="0" sqref="B312"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A238" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A244" activeCellId="0" sqref="A244"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.1377551020408"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="36.1785714285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.0969387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4728,9 +4725,9 @@
       <c r="E240" s="27"/>
       <c r="F240" s="27"/>
     </row>
-    <row r="241" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="241" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="26" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="B241" s="27" t="s">
         <v>264</v>
@@ -4742,9 +4739,9 @@
       <c r="E241" s="27"/>
       <c r="F241" s="27"/>
     </row>
-    <row r="242" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="242" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="26" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="B242" s="27" t="s">
         <v>266</v>
@@ -4756,9 +4753,9 @@
       <c r="E242" s="27"/>
       <c r="F242" s="27"/>
     </row>
-    <row r="243" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="243" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="26" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="B243" s="27" t="s">
         <v>268</v>
@@ -7575,7 +7572,7 @@
         <v>268</v>
       </c>
       <c r="C480" s="47" t="s">
-        <v>427</v>
+        <v>409</v>
       </c>
     </row>
     <row r="481" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7586,7 +7583,7 @@
         <v>268</v>
       </c>
       <c r="C481" s="47" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="482" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7597,7 +7594,7 @@
         <v>268</v>
       </c>
       <c r="C482" s="47" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="483" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7608,7 +7605,7 @@
         <v>268</v>
       </c>
       <c r="C483" s="47" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="484" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7619,7 +7616,7 @@
         <v>268</v>
       </c>
       <c r="C484" s="47" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="485" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7630,7 +7627,7 @@
         <v>268</v>
       </c>
       <c r="C485" s="47" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="486" customFormat="false" ht="22.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7641,7 +7638,7 @@
         <v>268</v>
       </c>
       <c r="C486" s="48" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="487" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7652,7 +7649,7 @@
         <v>303</v>
       </c>
       <c r="C487" s="47" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="488" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7674,7 +7671,7 @@
         <v>303</v>
       </c>
       <c r="C489" s="47" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="490" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7707,7 +7704,7 @@
         <v>303</v>
       </c>
       <c r="C492" s="47" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="493" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7718,7 +7715,7 @@
         <v>303</v>
       </c>
       <c r="C493" s="47" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="494" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7729,7 +7726,7 @@
         <v>303</v>
       </c>
       <c r="C494" s="47" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="495" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7751,7 +7748,7 @@
         <v>303</v>
       </c>
       <c r="C496" s="48" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="497" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7762,7 +7759,7 @@
         <v>316</v>
       </c>
       <c r="C497" s="47" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="498" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7784,7 +7781,7 @@
         <v>316</v>
       </c>
       <c r="C499" s="47" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="500" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7817,7 +7814,7 @@
         <v>316</v>
       </c>
       <c r="C502" s="47" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="503" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7828,7 +7825,7 @@
         <v>316</v>
       </c>
       <c r="C503" s="47" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="504" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7839,7 +7836,7 @@
         <v>316</v>
       </c>
       <c r="C504" s="47" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="505" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7861,7 +7858,7 @@
         <v>316</v>
       </c>
       <c r="C506" s="48" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="507" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7872,7 +7869,7 @@
         <v>320</v>
       </c>
       <c r="C507" s="47" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="508" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7883,7 +7880,7 @@
         <v>320</v>
       </c>
       <c r="C508" s="47" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="509" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7894,7 +7891,7 @@
         <v>320</v>
       </c>
       <c r="C509" s="47" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="510" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7905,7 +7902,7 @@
         <v>320</v>
       </c>
       <c r="C510" s="47" t="s">
-        <v>427</v>
+        <v>409</v>
       </c>
     </row>
     <row r="511" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7916,7 +7913,7 @@
         <v>320</v>
       </c>
       <c r="C511" s="47" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="512" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7927,7 +7924,7 @@
         <v>320</v>
       </c>
       <c r="C512" s="47" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="513" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7938,7 +7935,7 @@
         <v>320</v>
       </c>
       <c r="C513" s="47" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="514" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7949,7 +7946,7 @@
         <v>320</v>
       </c>
       <c r="C514" s="47" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="515" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7960,7 +7957,7 @@
         <v>320</v>
       </c>
       <c r="C515" s="47" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="516" customFormat="false" ht="22.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7971,7 +7968,7 @@
         <v>320</v>
       </c>
       <c r="C516" s="48" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="517" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7982,7 +7979,7 @@
         <v>6</v>
       </c>
       <c r="C517" s="47" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="518" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8004,7 +8001,7 @@
         <v>6</v>
       </c>
       <c r="C519" s="47" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="520" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8015,7 +8012,7 @@
         <v>6</v>
       </c>
       <c r="C520" s="47" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="521" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8026,7 +8023,7 @@
         <v>6</v>
       </c>
       <c r="C521" s="47" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="522" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8037,7 +8034,7 @@
         <v>6</v>
       </c>
       <c r="C522" s="47" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="523" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8048,7 +8045,7 @@
         <v>6</v>
       </c>
       <c r="C523" s="47" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="524" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8059,7 +8056,7 @@
         <v>6</v>
       </c>
       <c r="C524" s="47" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="525" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8070,7 +8067,7 @@
         <v>6</v>
       </c>
       <c r="C525" s="47" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="526" customFormat="false" ht="22.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8081,7 +8078,7 @@
         <v>6</v>
       </c>
       <c r="C526" s="48" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="527" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8092,7 +8089,7 @@
         <v>28</v>
       </c>
       <c r="C527" s="47" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="528" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8125,7 +8122,7 @@
         <v>28</v>
       </c>
       <c r="C530" s="47" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="531" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8136,7 +8133,7 @@
         <v>28</v>
       </c>
       <c r="C531" s="47" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="532" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8147,7 +8144,7 @@
         <v>28</v>
       </c>
       <c r="C532" s="47" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="533" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8169,7 +8166,7 @@
         <v>28</v>
       </c>
       <c r="C534" s="47" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="535" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8180,7 +8177,7 @@
         <v>28</v>
       </c>
       <c r="C535" s="47" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="536" customFormat="false" ht="22.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8191,7 +8188,7 @@
         <v>28</v>
       </c>
       <c r="C536" s="48" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="537" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Fixed bugs in read_excel.py made a function removed hardcoding of year, branch and filename-excel format should remain same
</commit_message>
<xml_diff>
--- a/Section-Faculty Information/subject_section_faculty_even_sem_2016.xlsx
+++ b/Section-Faculty Information/subject_section_faculty_even_sem_2016.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1599" uniqueCount="455">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1623" uniqueCount="456">
   <si>
     <t xml:space="preserve">EOE-081</t>
   </si>
@@ -1398,6 +1398,9 @@
   <si>
     <t xml:space="preserve">MR.SHUBHAM CHAUDHARY
 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ms.Pooja</t>
   </si>
 </sst>
 </file>
@@ -1504,10 +1507,9 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="11"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1524,7 +1526,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -1680,6 +1682,21 @@
       <bottom style="hair"/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FF313739"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF313739"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF313739"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF313739"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -1710,7 +1727,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="57">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1919,16 +1936,24 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="15" fillId="2" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="15" fillId="2" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1994,7 +2019,7 @@
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF313739"/>
       <rgbColor rgb="FF993300"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
@@ -2009,18 +2034,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:F538"/>
+  <dimension ref="A2:H545"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A238" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A244" activeCellId="0" sqref="A244"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A533" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C546" activeCellId="0" sqref="C546"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.5969387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.0969387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.3265306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.6938775510204"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8191,19 +8216,106 @@
         <v>454</v>
       </c>
     </row>
-    <row r="537" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A537" s="52"/>
-      <c r="B537" s="53"/>
-      <c r="C537" s="54"/>
-      <c r="D537" s="47"/>
-    </row>
-    <row r="538" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="539" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="540" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="541" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="542" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="543" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="544" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="537" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A537" s="52" t="s">
+        <v>61</v>
+      </c>
+      <c r="B537" s="0" t="s">
+        <v>293</v>
+      </c>
+      <c r="C537" s="53" t="s">
+        <v>113</v>
+      </c>
+      <c r="D537" s="54"/>
+      <c r="F537" s="55"/>
+      <c r="H537" s="56"/>
+    </row>
+    <row r="538" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A538" s="52" t="s">
+        <v>63</v>
+      </c>
+      <c r="B538" s="0" t="s">
+        <v>293</v>
+      </c>
+      <c r="C538" s="53" t="s">
+        <v>112</v>
+      </c>
+      <c r="D538" s="54"/>
+      <c r="F538" s="55"/>
+      <c r="H538" s="56"/>
+    </row>
+    <row r="539" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A539" s="52" t="s">
+        <v>64</v>
+      </c>
+      <c r="B539" s="0" t="s">
+        <v>293</v>
+      </c>
+      <c r="C539" s="52" t="s">
+        <v>114</v>
+      </c>
+      <c r="D539" s="54"/>
+      <c r="F539" s="55"/>
+      <c r="H539" s="56"/>
+    </row>
+    <row r="540" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A540" s="52" t="s">
+        <v>29</v>
+      </c>
+      <c r="B540" s="0" t="s">
+        <v>293</v>
+      </c>
+      <c r="C540" s="52" t="s">
+        <v>115</v>
+      </c>
+      <c r="D540" s="54"/>
+      <c r="F540" s="55"/>
+      <c r="H540" s="56"/>
+    </row>
+    <row r="541" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A541" s="52" t="s">
+        <v>61</v>
+      </c>
+      <c r="B541" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="C541" s="52" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="542" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A542" s="52" t="s">
+        <v>63</v>
+      </c>
+      <c r="B542" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="C542" s="52" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="543" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A543" s="52" t="s">
+        <v>64</v>
+      </c>
+      <c r="B543" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="C543" s="52" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="544" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A544" s="52" t="s">
+        <v>29</v>
+      </c>
+      <c r="B544" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="C544" s="52" t="s">
+        <v>122</v>
+      </c>
+    </row>
     <row r="545" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="546" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="547" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>